<commit_message>
Add linearity test results
</commit_message>
<xml_diff>
--- a/results/benchmarking-data.xlsx
+++ b/results/benchmarking-data.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="speed" sheetId="1" r:id="rId1"/>
     <sheet name="mpi" sheetId="2" r:id="rId2"/>
     <sheet name="mode" sheetId="3" r:id="rId3"/>
+    <sheet name="linear" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="25">
   <si>
     <t>g</t>
   </si>
@@ -1144,8 +1145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1636,4 +1637,255 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:H13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>100</v>
+      </c>
+      <c r="B4">
+        <v>0.01</v>
+      </c>
+      <c r="D4">
+        <v>100</v>
+      </c>
+      <c r="E4">
+        <v>0.01</v>
+      </c>
+      <c r="G4">
+        <v>100</v>
+      </c>
+      <c r="H4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1000</v>
+      </c>
+      <c r="B5">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="D5">
+        <v>1000</v>
+      </c>
+      <c r="E5">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="G5">
+        <v>1000</v>
+      </c>
+      <c r="H5">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>10000</v>
+      </c>
+      <c r="B6">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="D6">
+        <v>10000</v>
+      </c>
+      <c r="E6">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="G6">
+        <v>10000</v>
+      </c>
+      <c r="H6">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>100000</v>
+      </c>
+      <c r="B7">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="D7">
+        <v>100000</v>
+      </c>
+      <c r="E7">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="G7">
+        <v>100000</v>
+      </c>
+      <c r="H7">
+        <v>1.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1000000</v>
+      </c>
+      <c r="B8">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="D8">
+        <v>1000000</v>
+      </c>
+      <c r="E8">
+        <v>1.4E-2</v>
+      </c>
+      <c r="G8">
+        <v>1000000</v>
+      </c>
+      <c r="H8">
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>10000000</v>
+      </c>
+      <c r="B9">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="D9">
+        <v>10000000</v>
+      </c>
+      <c r="E9">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="G9">
+        <v>10000000</v>
+      </c>
+      <c r="H9">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>100000000</v>
+      </c>
+      <c r="B10">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="D10">
+        <v>100000000</v>
+      </c>
+      <c r="E10">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="G10">
+        <v>100000000</v>
+      </c>
+      <c r="H10">
+        <v>2.7170000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1000000000</v>
+      </c>
+      <c r="B11">
+        <v>9.2070000000000007</v>
+      </c>
+      <c r="D11">
+        <v>1000000000</v>
+      </c>
+      <c r="E11">
+        <v>5.6769999999999996</v>
+      </c>
+      <c r="G11">
+        <v>1000000000</v>
+      </c>
+      <c r="H11">
+        <v>27.117999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10000000000</v>
+      </c>
+      <c r="B12">
+        <v>91.863</v>
+      </c>
+      <c r="D12">
+        <v>10000000000</v>
+      </c>
+      <c r="E12">
+        <v>56.795999999999999</v>
+      </c>
+      <c r="G12">
+        <v>10000000000</v>
+      </c>
+      <c r="H12">
+        <v>267.94400000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>100000000000</v>
+      </c>
+      <c r="B13">
+        <v>876.14</v>
+      </c>
+      <c r="D13">
+        <v>100000000000</v>
+      </c>
+      <c r="E13">
+        <v>540.63499999999999</v>
+      </c>
+      <c r="G13">
+        <v>100000000000</v>
+      </c>
+      <c r="H13">
+        <v>2511.625</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>